<commit_message>
Added some more functionality
Added search loan application by loan id, changed send and reset password, resolved the date bug.
</commit_message>
<xml_diff>
--- a/Project Documents/Sample Bug Report.xlsx
+++ b/Project Documents/Sample Bug Report.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashparve\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manish Kumar\Documents\GitHub\FinanceProject\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465DAE55-13AC-42DB-9156-2981457FE4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAMPLE BUG REPORT" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Severity</t>
   </si>
@@ -60,12 +61,45 @@
   </si>
   <si>
     <t>Module</t>
+  </si>
+  <si>
+    <t>com.java.financeprojectapp.dataaccess.implementations</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Manish</t>
+  </si>
+  <si>
+    <t>Likhith</t>
+  </si>
+  <si>
+    <t>Insert a loan application and search using the frontend.</t>
+  </si>
+  <si>
+    <t>Loan Applications should be displayed</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Search by Date returns Null value. Mismatch between new Date(Long) and Date.valueOf(String)</t>
+  </si>
+  <si>
+    <t>DateBug</t>
+  </si>
+  <si>
+    <t>Check datebug in BugImages Folder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -415,23 +449,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="25.90625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.7265625" style="1"/>
     <col min="5" max="5" width="10.7265625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.36328125" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.26953125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="81.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30" style="1" customWidth="1"/>
     <col min="10" max="10" width="20.453125" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.7265625" style="1"/>
-    <col min="12" max="12" width="19.6328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -470,6 +507,41 @@
       </c>
       <c r="L1" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>